<commit_message>
Implemented POM design pattern in framework
</commit_message>
<xml_diff>
--- a/EdgeQA/InputSheet/UI_Codeless_Tests.xlsx
+++ b/EdgeQA/InputSheet/UI_Codeless_Tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\AI Project Workspace\Edge-Flow-QA\EdgeQA\InputSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\AI Project Workspace\Edge-Flow-QA\EdgeQA\inputSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70788949-9C02-4EE6-A258-23E7FEC00A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC325F6-190F-4EAB-A480-7E426054A395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>TC_UI_001</t>
+  </si>
+  <si>
+    <t>Create user</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TC_UI_002</t>
+  </si>
+  <si>
+    <t>Example domain flow</t>
+  </si>
+  <si>
+    <t>TC_UI_003</t>
+  </si>
+  <si>
+    <t>Navigation To Google and Searching</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>FlowName</t>
+  </si>
+  <si>
     <t>Step</t>
   </si>
   <si>
@@ -41,6 +77,9 @@
     <t>Expected</t>
   </si>
   <si>
+    <t>LOGIN_FLOW</t>
+  </si>
+  <si>
     <t>open_url</t>
   </si>
   <si>
@@ -50,112 +89,73 @@
     <t>fill_text</t>
   </si>
   <si>
+    <t>#username</t>
+  </si>
+  <si>
+    <t>{{username}}</t>
+  </si>
+  <si>
+    <t>#password</t>
+  </si>
+  <si>
+    <t>{{password}}</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>#loginBtn</t>
+  </si>
+  <si>
+    <t>LOGOUT_FLOW</t>
+  </si>
+  <si>
+    <t>#profile</t>
+  </si>
+  <si>
+    <t>#logout</t>
+  </si>
+  <si>
+    <t>OPEN_EXAMPLE_FLOW</t>
+  </si>
+  <si>
+    <t>https://example.com</t>
+  </si>
+  <si>
+    <t>CALL_FLOW</t>
+  </si>
+  <si>
+    <t>DashboardPage.addUser</t>
+  </si>
+  <si>
+    <t>DashboardPage.name</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>DashboardPage.save</t>
+  </si>
+  <si>
+    <t>assert_text</t>
+  </si>
+  <si>
+    <t>ExamplePage.title</t>
+  </si>
+  <si>
+    <t>Example Domain</t>
+  </si>
+  <si>
     <t>#APjFqb</t>
   </si>
   <si>
     <t>Xceedane pune</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
     <t>div[class='lJ9FBc'] input[name='btnK']</t>
   </si>
   <si>
     <t>#_L1WHadKuHKjd1e8P8piRmAE_44</t>
-  </si>
-  <si>
-    <t>TestCaseID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Execute</t>
-  </si>
-  <si>
-    <t>TC_UI_001</t>
-  </si>
-  <si>
-    <t>Create user</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>TC_UI_002</t>
-  </si>
-  <si>
-    <t>Example domain flow</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>TC_UI_003</t>
-  </si>
-  <si>
-    <t>Navigation To Google and Searching</t>
-  </si>
-  <si>
-    <t>FlowName</t>
-  </si>
-  <si>
-    <t>LOGIN_FLOW</t>
-  </si>
-  <si>
-    <t>#username</t>
-  </si>
-  <si>
-    <t>{{username}}</t>
-  </si>
-  <si>
-    <t>#password</t>
-  </si>
-  <si>
-    <t>{{password}}</t>
-  </si>
-  <si>
-    <t>#loginBtn</t>
-  </si>
-  <si>
-    <t>LOGOUT_FLOW</t>
-  </si>
-  <si>
-    <t>#profile</t>
-  </si>
-  <si>
-    <t>#logout</t>
-  </si>
-  <si>
-    <t>OPEN_EXAMPLE_FLOW</t>
-  </si>
-  <si>
-    <t>https://example.com</t>
-  </si>
-  <si>
-    <t>CALL_FLOW</t>
-  </si>
-  <si>
-    <t>#addUser</t>
-  </si>
-  <si>
-    <t>#name</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>#save</t>
-  </si>
-  <si>
-    <t>assert_text</t>
-  </si>
-  <si>
-    <t>h1</t>
-  </si>
-  <si>
-    <t>Example Domain</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -538,46 +538,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -604,136 +604,136 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -747,27 +747,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -775,10 +778,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -786,10 +789,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -797,13 +800,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,10 +814,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,10 +825,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -852,19 +855,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,10 +875,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -883,13 +886,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -914,19 +917,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -934,10 +937,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -947,13 +950,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -962,10 +965,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -975,10 +978,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>

</xml_diff>